<commit_message>
add read config flow
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UiPath\Project path\Amber_MuaHang_Vlookup\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JOB\RPA Project\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44489AD3-3B0D-4949-9065-A9F8F987C49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1ED636-FA3C-4E09-80AC-7D1AB68B4BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,42 +25,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>KEY</t>
   </si>
   <si>
-    <t>VALUE</t>
-  </si>
-  <si>
-    <t>usernameASP</t>
-  </si>
-  <si>
-    <t>passwordASP</t>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Birmingham, Manchester</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>Tuan@728</t>
   </si>
   <si>
-    <t>0906249919</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,7 +81,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -99,18 +97,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -392,23 +384,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -416,23 +407,35 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>906249919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{897A2366-F7C1-4CF2-9201-AE5CD00A8DB8}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{23F7ED15-0947-437E-A4B3-96A77DD27BDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chỉnh lại selector, thêm log
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UiPath\Project path\Amber_MuaHang_Vlookup\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9D7DB5-31A5-4BFF-B1C0-7080EF4A277C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A916E0-4D12-46CE-A85E-647D9CC77981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>usernameASP</t>
   </si>
   <si>
-    <t>D:\Documents\UiPath\Project path\Amber_MuaHang_Vlookup\Output\Danh muc NCC mau.xlsx</t>
+    <t>Output\Danh muc NCC mau.xlsx</t>
   </si>
 </sst>
 </file>
@@ -59,7 +59,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -67,7 +67,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -406,13 +406,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27.59765625" style="3" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -428,7 +428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -436,7 +436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
update lai version mới nhất
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49bfd0ea95b757c1/Documents/UiPath/RPA_AmberMuaHang/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{10A1C9E0-9F9D-464E-93CA-69C6AC4282D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFBC9DA1-18E1-4F63-A8EB-9CCFFF5A5592}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652ADA43-BD1D-4FE4-8812-242E22FBC2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3168" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>KEY</t>
   </si>
@@ -60,25 +60,22 @@
     <t>mhFileAddress</t>
   </si>
   <si>
+    <t>Output\Mua_hang_trong_nuoc.xls</t>
+  </si>
+  <si>
     <t>stage</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>dayUpdate</t>
   </si>
   <si>
-    <t>07/24/2023 16:34:52</t>
+    <t>07/28/2023 12:20:09</t>
   </si>
   <si>
     <t>uploadFolderName</t>
   </si>
   <si>
-    <t>24-07-2023</t>
-  </si>
-  <si>
-    <t>Output\Mua_hang_trong_nuoc.xls</t>
+    <t>28-07-2023</t>
   </si>
   <si>
     <t>usernameThue</t>
@@ -91,6 +88,18 @@
   </si>
   <si>
     <t>TCT@123</t>
+  </si>
+  <si>
+    <t>mailPhuTrach</t>
+  </si>
+  <si>
+    <t>kemclone1@gmail.com</t>
+  </si>
+  <si>
+    <t>mailKhachHang</t>
+  </si>
+  <si>
+    <t>kemclone3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -109,7 +118,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -164,10 +173,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,19 +461,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.19921875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -472,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -480,7 +489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -488,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -496,7 +505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -504,23 +513,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -528,7 +537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -536,27 +545,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="8" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa tên trường mail trong file config
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652ADA43-BD1D-4FE4-8812-242E22FBC2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB3FCC-22F7-4741-A6BE-816B684031FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2736" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>stage</t>
   </si>
   <si>
-    <t>dayUpdate</t>
-  </si>
-  <si>
     <t>07/28/2023 12:20:09</t>
   </si>
   <si>
@@ -96,10 +93,13 @@
     <t>kemclone1@gmail.com</t>
   </si>
   <si>
-    <t>mailKhachHang</t>
-  </si>
-  <si>
     <t>kemclone3@gmail.com</t>
+  </si>
+  <si>
+    <t>createdDay</t>
+  </si>
+  <si>
+    <t>mailAmber</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -526,55 +526,55 @@
         <v>12</v>
       </c>
       <c r="B7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thêm đường dẫn output NCC vào file config
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB3FCC-22F7-4741-A6BE-816B684031FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D61A817-49CA-4390-B035-67FD2124696C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>KEY</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>mailAmber</t>
+  </si>
+  <si>
+    <t>nccFileAddress</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -577,6 +580,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
sửa luồng tải từ vsign
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D61A817-49CA-4390-B035-67FD2124696C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E17753D-E444-4CDB-85AC-6B429617A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>KEY</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>nccFileAddress</t>
+  </si>
+  <si>
+    <t>maSoThue</t>
+  </si>
+  <si>
+    <t>0106777886</t>
   </si>
 </sst>
 </file>
@@ -159,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -183,6 +189,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -588,6 +597,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
sửa luồng tải từ vsign sửa lại drive
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\RPA_AmberMuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E17753D-E444-4CDB-85AC-6B429617A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B503F176-F106-47F3-9D3F-77B462024D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>KEY</t>
   </si>
@@ -66,13 +66,16 @@
     <t>stage</t>
   </si>
   <si>
-    <t>07/28/2023 12:20:09</t>
+    <t>createdDay</t>
+  </si>
+  <si>
+    <t>08/03/2023 10:14:47</t>
   </si>
   <si>
     <t>uploadFolderName</t>
   </si>
   <si>
-    <t>28-07-2023</t>
+    <t>DanhSachHHVT 03/08/2023</t>
   </si>
   <si>
     <t>usernameThue</t>
@@ -93,16 +96,10 @@
     <t>kemclone1@gmail.com</t>
   </si>
   <si>
+    <t>mailAmber</t>
+  </si>
+  <si>
     <t>kemclone3@gmail.com</t>
-  </si>
-  <si>
-    <t>createdDay</t>
-  </si>
-  <si>
-    <t>mailAmber</t>
-  </si>
-  <si>
-    <t>nccFileAddress</t>
   </si>
   <si>
     <t>maSoThue</t>
@@ -473,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -538,71 +535,63 @@
         <v>12</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bo sung file backup va sua dieu kien mo file vsign
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RPA_Amber_MuaHang\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D713633-00F0-47AB-85D2-3916227FC670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF98A8B-17FD-49A6-9A47-3C027F64FCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2604" yWindow="804" windowWidth="17820" windowHeight="11436" xr2:uid="{85067F95-7452-4B0E-89F8-0D85CF57B6E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85067F95-7452-4B0E-89F8-0D85CF57B6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>KEY</t>
   </si>
@@ -108,7 +108,25 @@
     <t>0106777886</t>
   </si>
   <si>
+    <t>vthhBackupFolder</t>
+  </si>
+  <si>
+    <t>BackupFileOutput\VTHH</t>
+  </si>
+  <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>nccBackupFolder</t>
+  </si>
+  <si>
+    <t>mhBackupFolder</t>
+  </si>
+  <si>
+    <t>BackupFileOutput\NCC</t>
+  </si>
+  <si>
+    <t>BackupFileOutput\MuaHang</t>
   </si>
 </sst>
 </file>
@@ -469,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB41FF8-57D3-47CD-BEBD-EFDC3C5A711D}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,7 +552,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -591,6 +609,30 @@
       </c>
       <c r="B14" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>